<commit_message>
Changes of 8th Sept 2023
</commit_message>
<xml_diff>
--- a/NetAgent/src/main/resources/NA OCP Result_STG.xlsx
+++ b/NetAgent/src/main/resources/NA OCP Result_STG.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="754" uniqueCount="105">
   <si>
     <t>Service</t>
   </si>
@@ -259,6 +259,140 @@
   </si>
   <si>
     <t>136871822</t>
+  </si>
+  <si>
+    <t>10276070</t>
+  </si>
+  <si>
+    <t>10276123</t>
+  </si>
+  <si>
+    <t>Cannot invoke "org.openqa.selenium.WebElement.isDisplayed()" because "element" is null</t>
+  </si>
+  <si>
+    <t>Cannot invoke "org.openqa.selenium.WebElement.getText()" because the return value of "connect_OCBaseMethods.TCAcknowledge.isElementPresent(String)" is null</t>
+  </si>
+  <si>
+    <t>javascript error: Cannot read properties of null (reading 'scrollIntoView')
+  (Session info: headless chrome=116.0.5845.142)
+Build info: version: '4.9.0', revision: 'd7057100a6'
+System info: os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '19.0.1'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Command: [042158f84f3375453d27a5b55d9cfdf3, executeScript {script=arguments[0].scrollIntoView();, args=[null]}]
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 116.0.5845.142, chrome: {chromedriverVersion: 116.0.5845.96 (1a3918166880..., userDataDir: C:\Users\RPRAJA~1\AppData\L...}, fedcm:accounts: true, goog:chromeOptions: {debuggerAddress: localhost:63951}, networkConnectionEnabled: false, pageLoadStrategy: normal, platformName: WINDOWS, proxy: Proxy(), se:cdp: ws://localhost:63951/devtoo..., se:cdpVersion: 116.0.5845.142, setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
+Session ID: 042158f84f3375453d27a5b55d9cfdf3</t>
+  </si>
+  <si>
+    <t>Cannot invoke "org.openqa.selenium.WebElement.getText()" because the return value of "connect_OrderProcessNonSPL.SDC.isElementPresent(String)" is null</t>
+  </si>
+  <si>
+    <t>no such element: Unable to locate element: {"method":"css selector","selector":"#lblServiceID"}
+  (Session info: headless chrome=116.0.5845.142)
+For documentation on this error, please visit: https://selenium.dev/exceptions/#no_such_element
+Build info: version: '4.9.0', revision: 'd7057100a6'
+System info: os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '19.0.1'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Command: [042158f84f3375453d27a5b55d9cfdf3, findElement {using=id, value=lblServiceID}]
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 116.0.5845.142, chrome: {chromedriverVersion: 116.0.5845.96 (1a3918166880..., userDataDir: C:\Users\RPRAJA~1\AppData\L...}, fedcm:accounts: true, goog:chromeOptions: {debuggerAddress: localhost:63951}, networkConnectionEnabled: false, pageLoadStrategy: normal, platformName: WINDOWS, proxy: Proxy(), se:cdp: ws://localhost:63951/devtoo..., se:cdpVersion: 116.0.5845.142, setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
+Session ID: 042158f84f3375453d27a5b55d9cfdf3</t>
+  </si>
+  <si>
+    <t>Expected condition failed: waiting for visibility of element located by By.id: a_tools (tried for 60 second(s) with 500 milliseconds interval)</t>
+  </si>
+  <si>
+    <t>Expected condition failed: waiting for visibility of element located by By.id: a_operations (tried for 50 second(s) with 500 milliseconds interval)</t>
+  </si>
+  <si>
+    <t>Expected condition failed: waiting for element to be clickable: By.id: idJobOverview (tried for 60 second(s) with 500 milliseconds interval)</t>
+  </si>
+  <si>
+    <t>10276189</t>
+  </si>
+  <si>
+    <t>10276200</t>
+  </si>
+  <si>
+    <t>10276217</t>
+  </si>
+  <si>
+    <t>10276250</t>
+  </si>
+  <si>
+    <t>javascript error: Cannot read properties of null (reading 'scrollIntoView')
+  (Session info: headless chrome=116.0.5845.142)
+Build info: version: '4.9.0', revision: 'd7057100a6'
+System info: os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '19.0.1'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Command: [d30b8ddfcd66d7e605a64e1e09fc7a3c, executeScript {script=arguments[0].scrollIntoView();, args=[null]}]
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 116.0.5845.142, chrome: {chromedriverVersion: 116.0.5845.96 (1a3918166880..., userDataDir: C:\Users\RPRAJA~1\AppData\L...}, fedcm:accounts: true, goog:chromeOptions: {debuggerAddress: localhost:49799}, networkConnectionEnabled: false, pageLoadStrategy: normal, platformName: WINDOWS, proxy: Proxy(), se:cdp: ws://localhost:49799/devtoo..., se:cdpVersion: 116.0.5845.142, setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
+Session ID: d30b8ddfcd66d7e605a64e1e09fc7a3c</t>
+  </si>
+  <si>
+    <t>no such element: Unable to locate element: {"method":"css selector","selector":"#lblServiceID"}
+  (Session info: headless chrome=116.0.5845.142)
+For documentation on this error, please visit: https://selenium.dev/exceptions/#no_such_element
+Build info: version: '4.9.0', revision: 'd7057100a6'
+System info: os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '19.0.1'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Command: [d30b8ddfcd66d7e605a64e1e09fc7a3c, findElement {using=id, value=lblServiceID}]
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 116.0.5845.142, chrome: {chromedriverVersion: 116.0.5845.96 (1a3918166880..., userDataDir: C:\Users\RPRAJA~1\AppData\L...}, fedcm:accounts: true, goog:chromeOptions: {debuggerAddress: localhost:49799}, networkConnectionEnabled: false, pageLoadStrategy: normal, platformName: WINDOWS, proxy: Proxy(), se:cdp: ws://localhost:49799/devtoo..., se:cdpVersion: 116.0.5845.142, setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
+Session ID: d30b8ddfcd66d7e605a64e1e09fc7a3c</t>
+  </si>
+  <si>
+    <t>10276268</t>
+  </si>
+  <si>
+    <t>10276301</t>
+  </si>
+  <si>
+    <t>10276307</t>
+  </si>
+  <si>
+    <t>10276322</t>
+  </si>
+  <si>
+    <t>10276342</t>
+  </si>
+  <si>
+    <t>10276348</t>
+  </si>
+  <si>
+    <t>10276357</t>
+  </si>
+  <si>
+    <t>10276377</t>
+  </si>
+  <si>
+    <t>10276394</t>
+  </si>
+  <si>
+    <t>794659437179</t>
+  </si>
+  <si>
+    <t>no such element: Unable to locate element: {"method":"css selector","selector":"#lblServiceID"}
+  (Session info: headless chrome=116.0.5845.142)
+For documentation on this error, please visit: https://selenium.dev/exceptions/#no_such_element
+Build info: version: '4.9.0', revision: 'd7057100a6'
+System info: os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '19.0.1'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Command: [a3777919d8494fa763fd310e1dbfa7ba, findElement {using=id, value=lblServiceID}]
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 116.0.5845.142, chrome: {chromedriverVersion: 116.0.5845.96 (1a3918166880..., userDataDir: C:\Users\RPRAJA~1\AppData\L...}, fedcm:accounts: true, goog:chromeOptions: {debuggerAddress: localhost:59939}, networkConnectionEnabled: false, pageLoadStrategy: normal, platformName: WINDOWS, proxy: Proxy(), se:cdp: ws://localhost:59939/devtoo..., se:cdpVersion: 116.0.5845.142, setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
+Session ID: a3777919d8494fa763fd310e1dbfa7ba</t>
+  </si>
+  <si>
+    <t>136919124</t>
+  </si>
+  <si>
+    <t>10276781</t>
+  </si>
+  <si>
+    <t>10276847</t>
+  </si>
+  <si>
+    <t>794659454491</t>
+  </si>
+  <si>
+    <t>10276859</t>
   </si>
 </sst>
 </file>
@@ -696,11 +830,11 @@
       </c>
       <c r="B2" s="1"/>
       <c r="C2" t="s">
-        <v>56</v>
+        <v>83</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="F2" t="s">
         <v>44</v>
@@ -714,11 +848,11 @@
       </c>
       <c r="B3" s="1"/>
       <c r="C3" t="s">
-        <v>57</v>
+        <v>84</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="F3" t="s">
         <v>44</v>
@@ -732,14 +866,14 @@
       </c>
       <c r="B4" s="1"/>
       <c r="C4" t="s">
-        <v>52</v>
+        <v>85</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="F4" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
@@ -750,11 +884,11 @@
       </c>
       <c r="B5" s="1"/>
       <c r="C5" t="s">
-        <v>59</v>
+        <v>89</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="F5" t="s">
         <v>44</v>
@@ -768,11 +902,11 @@
       </c>
       <c r="B6" s="1"/>
       <c r="C6" t="s">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="F6" t="s">
         <v>44</v>
@@ -786,11 +920,11 @@
       </c>
       <c r="B7" s="1"/>
       <c r="C7" t="s">
-        <v>61</v>
+        <v>91</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="F7" t="s">
         <v>44</v>
@@ -804,11 +938,11 @@
       </c>
       <c r="B8" s="1"/>
       <c r="C8" t="s">
-        <v>62</v>
+        <v>92</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="F8" t="s">
         <v>44</v>
@@ -822,11 +956,11 @@
       </c>
       <c r="B9" s="1"/>
       <c r="C9" t="s">
-        <v>63</v>
+        <v>93</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="F9" t="s">
         <v>44</v>
@@ -840,11 +974,11 @@
       </c>
       <c r="B10" s="1"/>
       <c r="C10" t="s">
-        <v>64</v>
+        <v>94</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="F10" t="s">
         <v>44</v>
@@ -858,14 +992,14 @@
       </c>
       <c r="B11" s="1"/>
       <c r="C11" t="s">
-        <v>65</v>
+        <v>95</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="F11" t="s">
-        <v>66</v>
+        <v>44</v>
       </c>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
@@ -876,14 +1010,14 @@
       </c>
       <c r="B12" s="1"/>
       <c r="C12" t="s">
-        <v>67</v>
+        <v>96</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="F12" t="s">
-        <v>68</v>
+        <v>44</v>
       </c>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
@@ -894,7 +1028,7 @@
       </c>
       <c r="B13" s="1"/>
       <c r="C13" t="s">
-        <v>69</v>
+        <v>102</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" t="s">
@@ -912,7 +1046,7 @@
       </c>
       <c r="B14" s="1"/>
       <c r="C14" t="s">
-        <v>71</v>
+        <v>104</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" t="s">
@@ -934,7 +1068,7 @@
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="F15" t="s">
         <v>44</v>
@@ -952,7 +1086,7 @@
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="F16" t="s">
         <v>44</v>
@@ -1022,7 +1156,7 @@
         <v>20</v>
       </c>
       <c r="C20" t="s">
-        <v>70</v>
+        <v>103</v>
       </c>
       <c r="D20" s="1"/>
       <c r="E20" t="s">
@@ -1096,11 +1230,11 @@
         <v>48</v>
       </c>
       <c r="C24" t="s">
-        <v>72</v>
+        <v>100</v>
       </c>
       <c r="D24" s="3"/>
       <c r="E24" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="F24" t="s">
         <v>44</v>
@@ -1116,7 +1250,7 @@
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
       <c r="E25" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="F25" t="s">
         <v>44</v>

</xml_diff>

<commit_message>
Changes of 5th oct 2023 OCP run upto D3P
</commit_message>
<xml_diff>
--- a/NetAgent/src/main/resources/NA OCP Result_STG.xlsx
+++ b/NetAgent/src/main/resources/NA OCP Result_STG.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3001" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3232" uniqueCount="275">
   <si>
     <t>Service</t>
   </si>
@@ -1048,6 +1048,67 @@
   </si>
   <si>
     <t>10329128</t>
+  </si>
+  <si>
+    <t>10331698</t>
+  </si>
+  <si>
+    <t>10331706</t>
+  </si>
+  <si>
+    <t>10331738</t>
+  </si>
+  <si>
+    <t>10331759</t>
+  </si>
+  <si>
+    <t>10331781</t>
+  </si>
+  <si>
+    <t>10331807</t>
+  </si>
+  <si>
+    <t>10331829</t>
+  </si>
+  <si>
+    <t>10331847</t>
+  </si>
+  <si>
+    <t>10331883</t>
+  </si>
+  <si>
+    <t>10331891</t>
+  </si>
+  <si>
+    <t>10331898</t>
+  </si>
+  <si>
+    <t>no such element: Unable to locate element: {"method":"css selector","selector":"#lblServiceID"}
+  (Session info: chrome=117.0.5938.132)
+For documentation on this error, please visit: https://www.seleniumhq.org/exceptions/no_such_element.html
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'SIPL92', ip: '10.212.130.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '19.0.1'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 117.0.5938.132, chrome: {chromedriverVersion: 117.0.5938.149 (e3344ddefa1..., userDataDir: C:\Users\RPRAJA~1\AppData\L...}, fedcm:accounts: true, goog:chromeOptions: {debuggerAddress: localhost:53317}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
+Session ID: 1e9fcc93b88024c6e34193c533e6edf3
+*** Element info: {Using=id, value=lblServiceID}</t>
+  </si>
+  <si>
+    <t>10331942</t>
+  </si>
+  <si>
+    <t>no such element: Unable to locate element: {"method":"css selector","selector":"#lblServiceID"}
+  (Session info: headless chrome=117.0.5938.132)
+For documentation on this error, please visit: https://www.seleniumhq.org/exceptions/no_such_element.html
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'SIPL92', ip: '10.212.130.15', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '19.0.1'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 117.0.5938.132, chrome: {chromedriverVersion: 117.0.5938.149 (e3344ddefa1..., userDataDir: C:\Users\RPRAJA~1\AppData\L...}, fedcm:accounts: true, goog:chromeOptions: {debuggerAddress: localhost:58444}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
+Session ID: d65df1f2c8a5d714bc9f8ba22fcbf8af
+*** Element info: {Using=id, value=lblServiceID}</t>
+  </si>
+  <si>
+    <t>10332023</t>
   </si>
 </sst>
 </file>
@@ -1435,7 +1496,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I26"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
@@ -1485,7 +1546,7 @@
       </c>
       <c r="B2" s="1"/>
       <c r="C2" t="s">
-        <v>255</v>
+        <v>260</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" t="s">
@@ -1503,7 +1564,7 @@
       </c>
       <c r="B3" s="1"/>
       <c r="C3" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" t="s">
@@ -1521,7 +1582,7 @@
       </c>
       <c r="B4" s="1"/>
       <c r="C4" t="s">
-        <v>257</v>
+        <v>262</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" t="s">
@@ -1539,7 +1600,7 @@
       </c>
       <c r="B5" s="1"/>
       <c r="C5" t="s">
-        <v>250</v>
+        <v>263</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" t="s">
@@ -1557,7 +1618,7 @@
       </c>
       <c r="B6" s="1"/>
       <c r="C6" t="s">
-        <v>242</v>
+        <v>264</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" t="s">
@@ -1575,7 +1636,7 @@
       </c>
       <c r="B7" s="1"/>
       <c r="C7" t="s">
-        <v>91</v>
+        <v>265</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" t="s">
@@ -1593,7 +1654,7 @@
       </c>
       <c r="B8" s="1"/>
       <c r="C8" t="s">
-        <v>243</v>
+        <v>266</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" t="s">
@@ -1611,7 +1672,7 @@
       </c>
       <c r="B9" s="1"/>
       <c r="C9" t="s">
-        <v>251</v>
+        <v>267</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" t="s">
@@ -1629,7 +1690,7 @@
       </c>
       <c r="B10" s="1"/>
       <c r="C10" t="s">
-        <v>245</v>
+        <v>268</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" t="s">
@@ -1647,7 +1708,7 @@
       </c>
       <c r="B11" s="1"/>
       <c r="C11" t="s">
-        <v>246</v>
+        <v>269</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" t="s">
@@ -1665,7 +1726,7 @@
       </c>
       <c r="B12" s="1"/>
       <c r="C12" t="s">
-        <v>226</v>
+        <v>274</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" t="s">
@@ -1723,7 +1784,7 @@
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="F15" t="s">
         <v>44</v>
@@ -1759,7 +1820,7 @@
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="F17" t="s">
         <v>44</v>
@@ -1777,7 +1838,7 @@
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="F18" t="s">
         <v>44</v>

</xml_diff>